<commit_message>
base finished chapter 6 95%
</commit_message>
<xml_diff>
--- a/autocrword/models/wind_f/工程量表/电气工程量表.xlsx
+++ b/autocrword/models/wind_f/工程量表/电气工程量表.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3EED1-99DD-41C3-8A09-1ABB076AA0A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="箱变容量选型表" sheetId="1" r:id="rId1"/>
     <sheet name="50MW设备选型" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
   <si>
     <t>2000</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1112,14 +1114,226 @@
       </rPr>
       <t xml:space="preserve">        0.2s/0.5s/5P30/5P30  5P30/5P30/5P30/5P30</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>型号</t>
+  </si>
+  <si>
+    <t>额定容量</t>
+  </si>
+  <si>
+    <t>额定电压比</t>
+  </si>
+  <si>
+    <t>接线组别</t>
+  </si>
+  <si>
+    <t>阻抗电压</t>
+  </si>
+  <si>
+    <t>冷却方式</t>
+  </si>
+  <si>
+    <t>SZ11-50000/110</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50MVA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>121±8×1.25%/37kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>YNd11</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ud=10.5%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ONAN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZ11-50000/220</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>232±8×1.25%/37kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ud=14%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>型式</t>
+  </si>
+  <si>
+    <t>额定电压</t>
+  </si>
+  <si>
+    <t>额定电流</t>
+  </si>
+  <si>
+    <t>额定频率</t>
+  </si>
+  <si>
+    <t>额定短时耐受电流</t>
+  </si>
+  <si>
+    <t>额定短路持续时间</t>
+  </si>
+  <si>
+    <t>额定峰值耐受电流</t>
+  </si>
+  <si>
+    <t>电流互感器变比</t>
+  </si>
+  <si>
+    <t>准确级</t>
+  </si>
+  <si>
+    <t>三相共箱式</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>126kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50Hz</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>40kA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3s</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>100kA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>300～600/1A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2s/0.5s/5P30/5P305P30/5P30/5P30/5P30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>三相分箱式</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>252kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50Hz</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50kA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3s</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>125kA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>300～600/1A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2s/0.5s/5P30/5P305P30/5P30/5P30/5P30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>避雷器额定电压（有效值）</t>
+  </si>
+  <si>
+    <t>避雷器持续运行电压(有效值)</t>
+  </si>
+  <si>
+    <t>避雷器的标称放电电流</t>
+  </si>
+  <si>
+    <t>雷电冲击电流残压（峰值）</t>
+  </si>
+  <si>
+    <t>方波通流容量峰值2ms、20次</t>
+  </si>
+  <si>
+    <t>氧化锌避雷器</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>204kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>152kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10kA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>532kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>800A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>氧化性避雷器</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>108kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>84kV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10kA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>281kV</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1190,6 +1404,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1283,9 +1504,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1297,6 +1515,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1318,7 +1539,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1393,6 +1614,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1428,6 +1666,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1603,11 +1858,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1619,7 +1874,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1630,7 +1885,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1641,7 +1896,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1652,7 +1907,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1663,7 +1918,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1674,7 +1929,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1685,7 +1940,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1703,11 +1958,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1715,11 +1970,11 @@
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="40.875" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1733,58 +1988,58 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>35</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="159" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>110</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="165" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>220</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1792,4 +2047,596 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B3E083-6D64-4E81-8D2A-866F94252649}">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2200</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2500</v>
+      </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2750</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3520</v>
+      </c>
+      <c r="L8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6">
+        <v>4000</v>
+      </c>
+      <c r="L9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" t="s">
+        <v>54</v>
+      </c>
+      <c r="O12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A13" s="11">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A14" s="11">
+        <v>220</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O15" t="s">
+        <v>48</v>
+      </c>
+      <c r="P15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A18" s="11">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A19" s="11">
+        <v>220</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" t="s">
+        <v>41</v>
+      </c>
+      <c r="P19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="L20" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O20" t="s">
+        <v>68</v>
+      </c>
+      <c r="P20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O21" t="s">
+        <v>69</v>
+      </c>
+      <c r="P21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" t="s">
+        <v>70</v>
+      </c>
+      <c r="M22" t="s">
+        <v>82</v>
+      </c>
+      <c r="O22" t="s">
+        <v>70</v>
+      </c>
+      <c r="P22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A23" s="11">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" t="s">
+        <v>83</v>
+      </c>
+      <c r="L23" t="s">
+        <v>71</v>
+      </c>
+      <c r="M23" t="s">
+        <v>83</v>
+      </c>
+      <c r="O23" t="s">
+        <v>71</v>
+      </c>
+      <c r="P23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A24" s="11">
+        <v>220</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+      <c r="O24" t="s">
+        <v>72</v>
+      </c>
+      <c r="P24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>